<commit_message>
Register User Usability Test commit
++ userability testcases
++ can only perform operations on elements with operations
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestExecution.xlsx
+++ b/src/test/resources/testdata/TestExecution.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Library\I - Jan - March Automation\HybridFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A740F89-CA59-4B03-964C-1507E82187A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E023D71-50EB-45F8-9C6E-572C307BD374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="316">
   <si>
     <t>Project Name</t>
   </si>
@@ -2632,13 +2632,88 @@
   </si>
   <si>
     <t>lethu@testautomation.co.za</t>
+  </si>
+  <si>
+    <t>//div[@id='firstname-error']</t>
+  </si>
+  <si>
+    <t>Nakith</t>
+  </si>
+  <si>
+    <t>Nuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuukithi</t>
+  </si>
+  <si>
+    <t>Mvuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuulo</t>
+  </si>
+  <si>
+    <t>_-q._.p-6</t>
+  </si>
+  <si>
+    <t>test7</t>
+  </si>
+  <si>
+    <t>VerifyPageUsabilityValidBlankFieldsTest</t>
+  </si>
+  <si>
+    <t>VerifyPageUsabilityPasswordMisMatchValidTest</t>
+  </si>
+  <si>
+    <t>VerifyPageUsabilityWeakPasswordValidTest</t>
+  </si>
+  <si>
+    <t>VerifyUsabilityWeakConfirmPasswordValidTest</t>
+  </si>
+  <si>
+    <t>VerifyUsabilityFieldRangeValidTest</t>
+  </si>
+  <si>
+    <t>lethu@testauuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuutomation.co.za</t>
+  </si>
+  <si>
+    <t>_-q._.p-7uuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuu</t>
+  </si>
+  <si>
+    <t>firstname-error</t>
+  </si>
+  <si>
+    <t>lastname-error</t>
+  </si>
+  <si>
+    <t>email-error</t>
+  </si>
+  <si>
+    <t>confirmpassword-error</t>
+  </si>
+  <si>
+    <t>//div[@id='password-confirmation-error']</t>
+  </si>
+  <si>
+    <t>//div[@id='password-strength-meter']</t>
+  </si>
+  <si>
+    <t>//div[@id='email_address-error']</t>
+  </si>
+  <si>
+    <t>//div[@id='lastname-error']</t>
+  </si>
+  <si>
+    <t>password-error</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2767,6 +2842,13 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3168,7 +3250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -3353,6 +3435,25 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3606,11 +3707,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3916,194 +4013,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B1" s="87"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="88"/>
-      <c r="O1" s="88"/>
-      <c r="P1" s="88"/>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
-      <c r="S1" s="88"/>
-      <c r="T1" s="88"/>
-      <c r="U1" s="88"/>
-      <c r="V1" s="88"/>
-      <c r="W1" s="88"/>
-      <c r="X1" s="89"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="95"/>
+      <c r="H1" s="95"/>
+      <c r="I1" s="95"/>
+      <c r="J1" s="95"/>
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+      <c r="M1" s="95"/>
+      <c r="N1" s="95"/>
+      <c r="O1" s="95"/>
+      <c r="P1" s="95"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="96"/>
     </row>
     <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B2" s="102"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-      <c r="P2" s="93"/>
-      <c r="Q2" s="93"/>
-      <c r="R2" s="93"/>
-      <c r="S2" s="93"/>
-      <c r="T2" s="93"/>
-      <c r="U2" s="93"/>
-      <c r="V2" s="93"/>
-      <c r="W2" s="93"/>
-      <c r="X2" s="103"/>
+      <c r="B2" s="109"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
+      <c r="L2" s="100"/>
+      <c r="M2" s="100"/>
+      <c r="N2" s="100"/>
+      <c r="O2" s="100"/>
+      <c r="P2" s="100"/>
+      <c r="Q2" s="100"/>
+      <c r="R2" s="100"/>
+      <c r="S2" s="100"/>
+      <c r="T2" s="100"/>
+      <c r="U2" s="100"/>
+      <c r="V2" s="100"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="110"/>
     </row>
     <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B3" s="102"/>
-      <c r="C3" s="93"/>
+      <c r="B3" s="109"/>
+      <c r="C3" s="100"/>
       <c r="W3" s="20"/>
       <c r="X3" s="30"/>
     </row>
     <row r="4" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="102"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="104" t="s">
+      <c r="B4" s="109"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="111" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
-      <c r="P4" s="105"/>
-      <c r="Q4" s="105"/>
-      <c r="R4" s="105"/>
-      <c r="S4" s="105"/>
-      <c r="T4" s="105"/>
-      <c r="U4" s="105"/>
-      <c r="V4" s="106"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="112"/>
+      <c r="Q4" s="112"/>
+      <c r="R4" s="112"/>
+      <c r="S4" s="112"/>
+      <c r="T4" s="112"/>
+      <c r="U4" s="112"/>
+      <c r="V4" s="113"/>
       <c r="W4" s="20"/>
       <c r="X4" s="30"/>
     </row>
     <row r="5" spans="2:24" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="102"/>
-      <c r="C5" s="93"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="110" t="s">
+      <c r="B5" s="109"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="117" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="110"/>
-      <c r="G5" s="110"/>
-      <c r="H5" s="110"/>
-      <c r="I5" s="110"/>
-      <c r="J5" s="110"/>
-      <c r="K5" s="110"/>
-      <c r="L5" s="110"/>
-      <c r="M5" s="110"/>
-      <c r="N5" s="110"/>
-      <c r="O5" s="110"/>
-      <c r="P5" s="110"/>
-      <c r="Q5" s="110"/>
-      <c r="R5" s="110"/>
-      <c r="S5" s="110"/>
-      <c r="T5" s="110"/>
-      <c r="U5" s="110"/>
-      <c r="V5" s="89"/>
+      <c r="F5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
+      <c r="R5" s="117"/>
+      <c r="S5" s="117"/>
+      <c r="T5" s="117"/>
+      <c r="U5" s="117"/>
+      <c r="V5" s="96"/>
       <c r="W5" s="20"/>
       <c r="X5" s="30"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B6" s="102"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="102"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="109"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
-      <c r="V6" s="103"/>
+      <c r="V6" s="110"/>
     </row>
     <row r="7" spans="2:24" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="102"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="111" t="s">
+      <c r="B7" s="109"/>
+      <c r="C7" s="100"/>
+      <c r="D7" s="109"/>
+      <c r="E7" s="118" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="111"/>
-      <c r="N7" s="111"/>
-      <c r="O7" s="111"/>
-      <c r="P7" s="111"/>
-      <c r="Q7" s="111"/>
-      <c r="R7" s="111"/>
-      <c r="S7" s="111"/>
-      <c r="T7" s="111"/>
-      <c r="U7" s="111"/>
-      <c r="V7" s="103"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="118"/>
+      <c r="Q7" s="118"/>
+      <c r="R7" s="118"/>
+      <c r="S7" s="118"/>
+      <c r="T7" s="118"/>
+      <c r="U7" s="118"/>
+      <c r="V7" s="110"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B8" s="102"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="90"/>
-      <c r="V8" s="92"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="97"/>
+      <c r="V8" s="99"/>
       <c r="W8" s="20"/>
       <c r="X8" s="30"/>
     </row>
     <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B9" s="102"/>
-      <c r="C9" s="93"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="100"/>
       <c r="D9" s="22"/>
-      <c r="E9" s="107" t="s">
+      <c r="E9" s="114" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="108"/>
-      <c r="G9" s="108"/>
-      <c r="H9" s="108"/>
-      <c r="I9" s="108"/>
-      <c r="J9" s="108"/>
-      <c r="K9" s="108"/>
-      <c r="L9" s="108"/>
-      <c r="M9" s="108"/>
-      <c r="N9" s="108"/>
-      <c r="O9" s="108"/>
-      <c r="P9" s="108"/>
-      <c r="Q9" s="108"/>
-      <c r="R9" s="108"/>
-      <c r="S9" s="108"/>
-      <c r="T9" s="108"/>
-      <c r="U9" s="109"/>
+      <c r="F9" s="115"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="115"/>
+      <c r="I9" s="115"/>
+      <c r="J9" s="115"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="115"/>
+      <c r="M9" s="115"/>
+      <c r="N9" s="115"/>
+      <c r="O9" s="115"/>
+      <c r="P9" s="115"/>
+      <c r="Q9" s="115"/>
+      <c r="R9" s="115"/>
+      <c r="S9" s="115"/>
+      <c r="T9" s="115"/>
+      <c r="U9" s="116"/>
       <c r="V9" s="24"/>
       <c r="W9" s="20"/>
       <c r="X9" s="30"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B10" s="102"/>
-      <c r="C10" s="93"/>
+      <c r="B10" s="109"/>
+      <c r="C10" s="100"/>
       <c r="D10" s="25"/>
       <c r="V10" s="26"/>
       <c r="W10" s="20"/>
       <c r="X10" s="30"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B11" s="102"/>
-      <c r="C11" s="93"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="100"/>
       <c r="D11" s="25"/>
       <c r="M11" s="1" t="s">
         <v>73</v>
@@ -4116,8 +4213,8 @@
       <c r="X11" s="30"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B12" s="102"/>
-      <c r="C12" s="93"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="100"/>
       <c r="D12" s="25"/>
       <c r="M12" s="1" t="s">
         <v>74</v>
@@ -4130,8 +4227,8 @@
       <c r="X12" s="30"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B13" s="102"/>
-      <c r="C13" s="93"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="100"/>
       <c r="D13" s="25"/>
       <c r="M13" s="1" t="s">
         <v>75</v>
@@ -4144,8 +4241,8 @@
       <c r="X13" s="30"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B14" s="102"/>
-      <c r="C14" s="93"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="100"/>
       <c r="D14" s="25"/>
       <c r="M14" s="1" t="s">
         <v>76</v>
@@ -4156,8 +4253,8 @@
       <c r="X14" s="30"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B15" s="102"/>
-      <c r="C15" s="93"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="100"/>
       <c r="D15" s="25"/>
       <c r="M15" s="6" t="s">
         <v>77</v>
@@ -4168,51 +4265,51 @@
       <c r="X15" s="30"/>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B16" s="102"/>
-      <c r="C16" s="93"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="100"/>
       <c r="D16" s="25"/>
       <c r="V16" s="26"/>
       <c r="W16" s="20"/>
       <c r="X16" s="30"/>
     </row>
     <row r="17" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="102"/>
-      <c r="C17" s="93"/>
-      <c r="D17" s="94" t="s">
+      <c r="B17" s="109"/>
+      <c r="C17" s="100"/>
+      <c r="D17" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="95"/>
-      <c r="F17" s="95"/>
-      <c r="G17" s="95"/>
-      <c r="H17" s="95"/>
-      <c r="I17" s="95"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="95"/>
-      <c r="L17" s="95"/>
-      <c r="M17" s="95"/>
-      <c r="N17" s="95"/>
-      <c r="O17" s="95"/>
-      <c r="P17" s="95"/>
-      <c r="Q17" s="95"/>
-      <c r="R17" s="95"/>
-      <c r="S17" s="95"/>
-      <c r="T17" s="95"/>
-      <c r="U17" s="95"/>
-      <c r="V17" s="96"/>
+      <c r="E17" s="102"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="102"/>
+      <c r="H17" s="102"/>
+      <c r="I17" s="102"/>
+      <c r="J17" s="102"/>
+      <c r="K17" s="102"/>
+      <c r="L17" s="102"/>
+      <c r="M17" s="102"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="102"/>
+      <c r="Q17" s="102"/>
+      <c r="R17" s="102"/>
+      <c r="S17" s="102"/>
+      <c r="T17" s="102"/>
+      <c r="U17" s="102"/>
+      <c r="V17" s="103"/>
       <c r="W17" s="20"/>
       <c r="X17" s="30"/>
     </row>
     <row r="18" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B18" s="102"/>
-      <c r="C18" s="93"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="100"/>
       <c r="D18" s="25"/>
       <c r="V18" s="26"/>
       <c r="W18" s="20"/>
       <c r="X18" s="30"/>
     </row>
     <row r="19" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B19" s="102"/>
-      <c r="C19" s="93"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="100"/>
       <c r="D19" s="25"/>
       <c r="F19" s="1" t="s">
         <v>81</v>
@@ -4237,8 +4334,8 @@
       <c r="X19" s="30"/>
     </row>
     <row r="20" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B20" s="102"/>
-      <c r="C20" s="93"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="100"/>
       <c r="D20" s="25"/>
       <c r="F20" s="1" t="s">
         <v>82</v>
@@ -4257,8 +4354,8 @@
       <c r="X20" s="30"/>
     </row>
     <row r="21" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B21" s="102"/>
-      <c r="C21" s="93"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="100"/>
       <c r="D21" s="25"/>
       <c r="F21" s="21" t="s">
         <v>83</v>
@@ -4283,8 +4380,8 @@
       <c r="X21" s="30"/>
     </row>
     <row r="22" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B22" s="102"/>
-      <c r="C22" s="93"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="100"/>
       <c r="D22" s="25"/>
       <c r="F22" s="1" t="s">
         <v>76</v>
@@ -4303,8 +4400,8 @@
       <c r="X22" s="30"/>
     </row>
     <row r="23" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B23" s="102"/>
-      <c r="C23" s="93"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="100"/>
       <c r="D23" s="25"/>
       <c r="F23" s="6" t="s">
         <v>77</v>
@@ -4323,16 +4420,16 @@
       <c r="X23" s="30"/>
     </row>
     <row r="24" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B24" s="102"/>
-      <c r="C24" s="93"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="100"/>
       <c r="D24" s="25"/>
       <c r="V24" s="26"/>
       <c r="W24" s="20"/>
       <c r="X24" s="30"/>
     </row>
     <row r="25" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B25" s="102"/>
-      <c r="C25" s="93"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="27"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
@@ -4356,52 +4453,52 @@
       <c r="X25" s="30"/>
     </row>
     <row r="26" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B26" s="102"/>
-      <c r="C26" s="93"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88"/>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88"/>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88"/>
-      <c r="N26" s="88"/>
-      <c r="O26" s="88"/>
-      <c r="P26" s="88"/>
-      <c r="Q26" s="88"/>
-      <c r="R26" s="88"/>
-      <c r="S26" s="88"/>
-      <c r="T26" s="88"/>
-      <c r="U26" s="88"/>
-      <c r="V26" s="88"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="95"/>
+      <c r="M26" s="95"/>
+      <c r="N26" s="95"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="95"/>
+      <c r="U26" s="95"/>
+      <c r="V26" s="95"/>
       <c r="W26" s="20"/>
       <c r="X26" s="30"/>
     </row>
     <row r="27" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B27" s="90"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="91"/>
-      <c r="P27" s="91"/>
-      <c r="Q27" s="91"/>
-      <c r="R27" s="91"/>
-      <c r="S27" s="91"/>
-      <c r="T27" s="91"/>
-      <c r="U27" s="91"/>
-      <c r="V27" s="91"/>
+      <c r="B27" s="97"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="98"/>
+      <c r="J27" s="98"/>
+      <c r="K27" s="98"/>
+      <c r="L27" s="98"/>
+      <c r="M27" s="98"/>
+      <c r="N27" s="98"/>
+      <c r="O27" s="98"/>
+      <c r="P27" s="98"/>
+      <c r="Q27" s="98"/>
+      <c r="R27" s="98"/>
+      <c r="S27" s="98"/>
+      <c r="T27" s="98"/>
+      <c r="U27" s="98"/>
+      <c r="V27" s="98"/>
       <c r="W27" s="31"/>
       <c r="X27" s="32"/>
     </row>
@@ -4432,131 +4529,131 @@
     </row>
     <row r="29" spans="2:24" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B29" s="25"/>
-      <c r="G29" s="94" t="s">
+      <c r="G29" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="H29" s="95"/>
-      <c r="I29" s="95"/>
-      <c r="J29" s="95"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="95"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="95"/>
-      <c r="O29" s="95"/>
-      <c r="P29" s="95"/>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="95"/>
-      <c r="S29" s="95"/>
-      <c r="T29" s="96"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="102"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="102"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="102"/>
+      <c r="T29" s="103"/>
       <c r="X29" s="26"/>
     </row>
     <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="25"/>
-      <c r="G30" s="87"/>
-      <c r="H30" s="98" t="s">
+      <c r="G30" s="94"/>
+      <c r="H30" s="105" t="s">
         <v>87</v>
       </c>
-      <c r="I30" s="98"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="98"/>
-      <c r="M30" s="97" t="s">
+      <c r="I30" s="105"/>
+      <c r="J30" s="105"/>
+      <c r="K30" s="105"/>
+      <c r="M30" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="N30" s="97"/>
-      <c r="O30" s="98" t="s">
+      <c r="N30" s="104"/>
+      <c r="O30" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="P30" s="98"/>
-      <c r="Q30" s="98"/>
-      <c r="R30" s="98"/>
-      <c r="S30" s="98"/>
-      <c r="T30" s="89"/>
+      <c r="P30" s="105"/>
+      <c r="Q30" s="105"/>
+      <c r="R30" s="105"/>
+      <c r="S30" s="105"/>
+      <c r="T30" s="96"/>
       <c r="X30" s="26"/>
     </row>
     <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="25"/>
-      <c r="G31" s="102"/>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
-      <c r="K31" s="93"/>
-      <c r="M31" s="93"/>
-      <c r="N31" s="93"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="93"/>
-      <c r="Q31" s="93"/>
-      <c r="R31" s="93"/>
-      <c r="S31" s="93"/>
-      <c r="T31" s="103"/>
+      <c r="G31" s="109"/>
+      <c r="H31" s="100"/>
+      <c r="I31" s="100"/>
+      <c r="J31" s="100"/>
+      <c r="K31" s="100"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="100"/>
+      <c r="S31" s="100"/>
+      <c r="T31" s="110"/>
       <c r="X31" s="26"/>
     </row>
     <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B32" s="25"/>
-      <c r="G32" s="102"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="93"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="93"/>
-      <c r="Q32" s="93"/>
-      <c r="R32" s="93"/>
-      <c r="S32" s="93"/>
-      <c r="T32" s="103"/>
+      <c r="G32" s="109"/>
+      <c r="H32" s="100"/>
+      <c r="I32" s="100"/>
+      <c r="J32" s="100"/>
+      <c r="K32" s="100"/>
+      <c r="M32" s="100"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="100"/>
+      <c r="P32" s="100"/>
+      <c r="Q32" s="100"/>
+      <c r="R32" s="100"/>
+      <c r="S32" s="100"/>
+      <c r="T32" s="110"/>
       <c r="X32" s="26"/>
     </row>
     <row r="33" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B33" s="25"/>
-      <c r="G33" s="102"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="M33" s="93"/>
-      <c r="N33" s="93"/>
-      <c r="O33" s="93"/>
-      <c r="P33" s="93"/>
-      <c r="Q33" s="93"/>
-      <c r="R33" s="93"/>
-      <c r="S33" s="93"/>
-      <c r="T33" s="103"/>
+      <c r="G33" s="109"/>
+      <c r="H33" s="100"/>
+      <c r="I33" s="100"/>
+      <c r="J33" s="100"/>
+      <c r="K33" s="100"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="100"/>
+      <c r="Q33" s="100"/>
+      <c r="R33" s="100"/>
+      <c r="S33" s="100"/>
+      <c r="T33" s="110"/>
       <c r="X33" s="26"/>
     </row>
     <row r="34" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B34" s="25"/>
-      <c r="G34" s="90"/>
-      <c r="H34" s="91"/>
-      <c r="I34" s="91"/>
-      <c r="J34" s="91"/>
-      <c r="K34" s="91"/>
-      <c r="M34" s="91"/>
-      <c r="N34" s="91"/>
-      <c r="O34" s="91"/>
-      <c r="P34" s="91"/>
-      <c r="Q34" s="91"/>
-      <c r="R34" s="91"/>
-      <c r="S34" s="91"/>
-      <c r="T34" s="92"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="98"/>
+      <c r="I34" s="98"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="98"/>
+      <c r="M34" s="98"/>
+      <c r="N34" s="98"/>
+      <c r="O34" s="98"/>
+      <c r="P34" s="98"/>
+      <c r="Q34" s="98"/>
+      <c r="R34" s="98"/>
+      <c r="S34" s="98"/>
+      <c r="T34" s="99"/>
       <c r="X34" s="26"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B35" s="25"/>
-      <c r="G35" s="99"/>
-      <c r="H35" s="100"/>
-      <c r="I35" s="100"/>
-      <c r="J35" s="100"/>
-      <c r="K35" s="100"/>
-      <c r="L35" s="100"/>
-      <c r="M35" s="100"/>
-      <c r="N35" s="100"/>
-      <c r="O35" s="100"/>
-      <c r="P35" s="100"/>
-      <c r="Q35" s="100"/>
-      <c r="R35" s="100"/>
-      <c r="S35" s="100"/>
-      <c r="T35" s="101"/>
+      <c r="G35" s="106"/>
+      <c r="H35" s="107"/>
+      <c r="I35" s="107"/>
+      <c r="J35" s="107"/>
+      <c r="K35" s="107"/>
+      <c r="L35" s="107"/>
+      <c r="M35" s="107"/>
+      <c r="N35" s="107"/>
+      <c r="O35" s="107"/>
+      <c r="P35" s="107"/>
+      <c r="Q35" s="107"/>
+      <c r="R35" s="107"/>
+      <c r="S35" s="107"/>
+      <c r="T35" s="108"/>
       <c r="X35" s="26"/>
     </row>
     <row r="36" spans="2:24" x14ac:dyDescent="0.25">
@@ -4565,73 +4662,73 @@
     </row>
     <row r="37" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B37" s="25"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="88"/>
-      <c r="G37" s="88"/>
-      <c r="H37" s="88"/>
-      <c r="I37" s="88"/>
-      <c r="J37" s="88"/>
-      <c r="K37" s="88"/>
-      <c r="L37" s="88"/>
-      <c r="M37" s="88"/>
-      <c r="N37" s="88"/>
-      <c r="O37" s="88"/>
-      <c r="P37" s="88"/>
-      <c r="Q37" s="88"/>
-      <c r="R37" s="88"/>
-      <c r="S37" s="88"/>
-      <c r="T37" s="88"/>
-      <c r="U37" s="88"/>
-      <c r="V37" s="89"/>
+      <c r="D37" s="94"/>
+      <c r="E37" s="95"/>
+      <c r="F37" s="95"/>
+      <c r="G37" s="95"/>
+      <c r="H37" s="95"/>
+      <c r="I37" s="95"/>
+      <c r="J37" s="95"/>
+      <c r="K37" s="95"/>
+      <c r="L37" s="95"/>
+      <c r="M37" s="95"/>
+      <c r="N37" s="95"/>
+      <c r="O37" s="95"/>
+      <c r="P37" s="95"/>
+      <c r="Q37" s="95"/>
+      <c r="R37" s="95"/>
+      <c r="S37" s="95"/>
+      <c r="T37" s="95"/>
+      <c r="U37" s="95"/>
+      <c r="V37" s="96"/>
       <c r="X37" s="26"/>
     </row>
     <row r="38" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B38" s="25"/>
       <c r="D38" s="25"/>
-      <c r="E38" s="84" t="s">
+      <c r="E38" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="85"/>
-      <c r="G38" s="85"/>
-      <c r="H38" s="85"/>
-      <c r="I38" s="85"/>
-      <c r="J38" s="85"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="85"/>
-      <c r="M38" s="85"/>
-      <c r="N38" s="85"/>
-      <c r="O38" s="85"/>
-      <c r="P38" s="85"/>
-      <c r="Q38" s="85"/>
-      <c r="R38" s="85"/>
-      <c r="S38" s="85"/>
-      <c r="T38" s="85"/>
-      <c r="U38" s="86"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="92"/>
+      <c r="I38" s="92"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="92"/>
+      <c r="L38" s="92"/>
+      <c r="M38" s="92"/>
+      <c r="N38" s="92"/>
+      <c r="O38" s="92"/>
+      <c r="P38" s="92"/>
+      <c r="Q38" s="92"/>
+      <c r="R38" s="92"/>
+      <c r="S38" s="92"/>
+      <c r="T38" s="92"/>
+      <c r="U38" s="93"/>
       <c r="V38" s="26"/>
       <c r="X38" s="26"/>
     </row>
     <row r="39" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B39" s="25"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="91"/>
-      <c r="F39" s="91"/>
-      <c r="G39" s="91"/>
-      <c r="H39" s="91"/>
-      <c r="I39" s="91"/>
-      <c r="J39" s="91"/>
-      <c r="K39" s="91"/>
-      <c r="L39" s="91"/>
-      <c r="M39" s="91"/>
-      <c r="N39" s="91"/>
-      <c r="O39" s="91"/>
-      <c r="P39" s="91"/>
-      <c r="Q39" s="91"/>
-      <c r="R39" s="91"/>
-      <c r="S39" s="91"/>
-      <c r="T39" s="91"/>
-      <c r="U39" s="91"/>
-      <c r="V39" s="92"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="98"/>
+      <c r="F39" s="98"/>
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
+      <c r="L39" s="98"/>
+      <c r="M39" s="98"/>
+      <c r="N39" s="98"/>
+      <c r="O39" s="98"/>
+      <c r="P39" s="98"/>
+      <c r="Q39" s="98"/>
+      <c r="R39" s="98"/>
+      <c r="S39" s="98"/>
+      <c r="T39" s="98"/>
+      <c r="U39" s="98"/>
+      <c r="V39" s="99"/>
       <c r="X39" s="26"/>
     </row>
     <row r="40" spans="2:24" x14ac:dyDescent="0.25">
@@ -4772,19 +4869,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -5261,8 +5358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A60A778-2A5D-4CCB-968B-7363B04FA1F7}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5315,17 +5412,17 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="174" t="s">
         <v>249</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
       <c r="J2" s="8"/>
       <c r="K2" s="7"/>
     </row>
@@ -5745,19 +5842,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">
@@ -6019,7 +6116,7 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F3" location="'User Details Usability'!A1" display="Registration &amp; Login - Usability Checklist" xr:uid="{3CD879B6-DA4C-4CA8-BF76-EAF867966A62}"/>
-    <hyperlink ref="A2:K2" location="'Register Test Scenarios'!A1" display="Test sceanrios" xr:uid="{4BD8A3C2-A963-4F3C-9F41-68DDAC13EA3C}"/>
+    <hyperlink ref="A2:K2" location="'Test Scenarios'!A1" display="Test sceanrios" xr:uid="{4BD8A3C2-A963-4F3C-9F41-68DDAC13EA3C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6085,19 +6182,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -6238,19 +6335,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -6390,19 +6487,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -6542,19 +6639,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -6696,19 +6793,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -6850,19 +6947,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -7005,19 +7102,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="168" t="s">
+      <c r="A2" s="175" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="169"/>
-      <c r="C2" s="169"/>
-      <c r="D2" s="169"/>
-      <c r="E2" s="169"/>
-      <c r="F2" s="169"/>
-      <c r="G2" s="169"/>
-      <c r="H2" s="169"/>
-      <c r="I2" s="169"/>
-      <c r="J2" s="169"/>
-      <c r="K2" s="170"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
+      <c r="K2" s="177"/>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -7125,47 +7222,47 @@
         <v>0</v>
       </c>
       <c r="B1" s="26"/>
-      <c r="C1" s="124" t="s">
+      <c r="C1" s="131" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="125"/>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125"/>
-      <c r="H1" s="125"/>
-      <c r="I1" s="125"/>
-      <c r="J1" s="125"/>
-      <c r="K1" s="126"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="133"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3"/>
-      <c r="C2" s="127"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="129"/>
+      <c r="C2" s="134"/>
+      <c r="D2" s="135"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="135"/>
+      <c r="G2" s="135"/>
+      <c r="H2" s="135"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="135"/>
+      <c r="K2" s="136"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2"/>
-      <c r="C3" s="127"/>
-      <c r="D3" s="128"/>
-      <c r="E3" s="128"/>
-      <c r="F3" s="128"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="128"/>
-      <c r="K3" s="129"/>
+      <c r="C3" s="134"/>
+      <c r="D3" s="135"/>
+      <c r="E3" s="135"/>
+      <c r="F3" s="135"/>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135"/>
+      <c r="K3" s="136"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -7174,225 +7271,225 @@
       <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="127"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="128"/>
-      <c r="F4" s="128"/>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="129"/>
+      <c r="C4" s="134"/>
+      <c r="D4" s="135"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="135"/>
+      <c r="K4" s="136"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="127"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="128"/>
-      <c r="F5" s="128"/>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="129"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="136"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="127"/>
-      <c r="D6" s="128"/>
-      <c r="E6" s="128"/>
-      <c r="F6" s="128"/>
-      <c r="G6" s="128"/>
-      <c r="H6" s="128"/>
-      <c r="I6" s="128"/>
-      <c r="J6" s="128"/>
-      <c r="K6" s="129"/>
+      <c r="C6" s="134"/>
+      <c r="D6" s="135"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="136"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="127"/>
-      <c r="D7" s="128"/>
-      <c r="E7" s="128"/>
-      <c r="F7" s="128"/>
-      <c r="G7" s="128"/>
-      <c r="H7" s="128"/>
-      <c r="I7" s="128"/>
-      <c r="J7" s="128"/>
-      <c r="K7" s="129"/>
+      <c r="A7" s="95"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="134"/>
+      <c r="D7" s="135"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="136"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="91"/>
-      <c r="B8" s="92"/>
-      <c r="C8" s="130"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="131"/>
-      <c r="G8" s="131"/>
-      <c r="H8" s="131"/>
-      <c r="I8" s="131"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="132"/>
+      <c r="A8" s="98"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="137"/>
+      <c r="D8" s="138"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="139"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="87"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="88"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="88"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
-      <c r="K9" s="88"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="95"/>
+      <c r="C9" s="95"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="95"/>
+      <c r="H9" s="95"/>
+      <c r="I9" s="95"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="90"/>
-      <c r="B10" s="91"/>
-      <c r="C10" s="91"/>
-      <c r="D10" s="91"/>
-      <c r="E10" s="91"/>
+      <c r="A10" s="97"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="139"/>
-      <c r="H10" s="139"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="119" t="s">
+      <c r="G10" s="146"/>
+      <c r="H10" s="146"/>
+      <c r="I10" s="147"/>
+      <c r="J10" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="K10" s="120"/>
+      <c r="K10" s="127"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="133" t="s">
+      <c r="A11" s="140" t="s">
         <v>96</v>
       </c>
-      <c r="B11" s="134"/>
-      <c r="C11" s="134"/>
-      <c r="D11" s="134"/>
-      <c r="E11" s="135"/>
-      <c r="G11" s="133" t="s">
+      <c r="B11" s="141"/>
+      <c r="C11" s="141"/>
+      <c r="D11" s="141"/>
+      <c r="E11" s="142"/>
+      <c r="G11" s="140" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="135"/>
+      <c r="H11" s="141"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="142"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="116" t="s">
+      <c r="B12" s="123" t="s">
         <v>99</v>
       </c>
-      <c r="C12" s="117"/>
-      <c r="D12" s="117"/>
-      <c r="E12" s="118"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="114"/>
+      <c r="C12" s="124"/>
+      <c r="D12" s="124"/>
+      <c r="E12" s="125"/>
+      <c r="G12" s="94"/>
+      <c r="H12" s="95"/>
+      <c r="I12" s="95"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="121"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="116" t="s">
+      <c r="B13" s="123" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
-      <c r="E13" s="118"/>
-      <c r="G13" s="102"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="103"/>
-      <c r="K13" s="114"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="124"/>
+      <c r="E13" s="125"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="100"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="121"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="116" t="s">
+      <c r="B14" s="123" t="s">
         <v>100</v>
       </c>
-      <c r="C14" s="117"/>
-      <c r="D14" s="117"/>
-      <c r="E14" s="118"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="93"/>
-      <c r="I14" s="93"/>
-      <c r="J14" s="103"/>
-      <c r="K14" s="114"/>
+      <c r="C14" s="124"/>
+      <c r="D14" s="124"/>
+      <c r="E14" s="125"/>
+      <c r="G14" s="109"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="100"/>
+      <c r="J14" s="110"/>
+      <c r="K14" s="121"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="116" t="s">
+      <c r="B15" s="123" t="s">
         <v>102</v>
       </c>
-      <c r="C15" s="117"/>
-      <c r="D15" s="117"/>
-      <c r="E15" s="118"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="103"/>
-      <c r="K15" s="114"/>
+      <c r="C15" s="124"/>
+      <c r="D15" s="124"/>
+      <c r="E15" s="125"/>
+      <c r="G15" s="109"/>
+      <c r="H15" s="100"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="110"/>
+      <c r="K15" s="121"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="116" t="s">
+      <c r="B16" s="123" t="s">
         <v>101</v>
       </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="117"/>
-      <c r="E16" s="118"/>
-      <c r="G16" s="90"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="92"/>
-      <c r="K16" s="114"/>
+      <c r="C16" s="124"/>
+      <c r="D16" s="124"/>
+      <c r="E16" s="125"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="98"/>
+      <c r="I16" s="98"/>
+      <c r="J16" s="99"/>
+      <c r="K16" s="121"/>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="119" t="s">
+      <c r="D18" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="120"/>
-      <c r="G18" s="91"/>
-      <c r="H18" s="91"/>
-      <c r="I18" s="141"/>
-      <c r="J18" s="119" t="s">
+      <c r="E18" s="127"/>
+      <c r="G18" s="98"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="K18" s="138"/>
+      <c r="K18" s="145"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="121" t="s">
+      <c r="A19" s="128" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="134"/>
-      <c r="E19" s="142"/>
-      <c r="G19" s="121" t="s">
+      <c r="B19" s="129"/>
+      <c r="C19" s="129"/>
+      <c r="D19" s="141"/>
+      <c r="E19" s="149"/>
+      <c r="G19" s="128" t="s">
         <v>106</v>
       </c>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
-      <c r="J19" s="134"/>
-      <c r="K19" s="135"/>
+      <c r="H19" s="129"/>
+      <c r="I19" s="129"/>
+      <c r="J19" s="141"/>
+      <c r="K19" s="142"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
@@ -7404,7 +7501,7 @@
       <c r="C20" t="s">
         <v>118</v>
       </c>
-      <c r="E20" s="115"/>
+      <c r="E20" s="122"/>
       <c r="G20" s="41" t="s">
         <v>110</v>
       </c>
@@ -7414,7 +7511,7 @@
       <c r="I20" t="s">
         <v>118</v>
       </c>
-      <c r="K20" s="114"/>
+      <c r="K20" s="121"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -7426,7 +7523,7 @@
       <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="E21" s="115"/>
+      <c r="E21" s="122"/>
       <c r="G21" t="s">
         <v>111</v>
       </c>
@@ -7436,7 +7533,7 @@
       <c r="I21" t="s">
         <v>117</v>
       </c>
-      <c r="K21" s="114"/>
+      <c r="K21" s="121"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
@@ -7448,7 +7545,7 @@
       <c r="C22" t="s">
         <v>116</v>
       </c>
-      <c r="E22" s="115"/>
+      <c r="E22" s="122"/>
       <c r="G22" s="25" t="s">
         <v>109</v>
       </c>
@@ -7458,7 +7555,7 @@
       <c r="I22" t="s">
         <v>116</v>
       </c>
-      <c r="K22" s="114"/>
+      <c r="K22" s="121"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
@@ -7470,7 +7567,7 @@
       <c r="C23" t="s">
         <v>115</v>
       </c>
-      <c r="E23" s="115"/>
+      <c r="E23" s="122"/>
       <c r="G23" s="25" t="s">
         <v>113</v>
       </c>
@@ -7480,7 +7577,7 @@
       <c r="I23" t="s">
         <v>115</v>
       </c>
-      <c r="K23" s="114"/>
+      <c r="K23" s="121"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="27" t="s">
@@ -7491,7 +7588,7 @@
       </c>
       <c r="C24" s="28"/>
       <c r="D24" s="28"/>
-      <c r="E24" s="115"/>
+      <c r="E24" s="122"/>
       <c r="G24" s="27" t="s">
         <v>122</v>
       </c>
@@ -7500,37 +7597,37 @@
       </c>
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
-      <c r="K24" s="114"/>
+      <c r="K24" s="121"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="136" t="s">
+      <c r="D26" s="143" t="s">
         <v>97</v>
       </c>
-      <c r="E26" s="137"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="141"/>
-      <c r="J26" s="119" t="s">
+      <c r="E26" s="144"/>
+      <c r="G26" s="98"/>
+      <c r="H26" s="98"/>
+      <c r="I26" s="148"/>
+      <c r="J26" s="126" t="s">
         <v>97</v>
       </c>
-      <c r="K26" s="138"/>
+      <c r="K26" s="145"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="128" t="s">
         <v>104</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="122"/>
-      <c r="D27" s="122"/>
-      <c r="E27" s="123"/>
-      <c r="G27" s="121" t="s">
+      <c r="B27" s="129"/>
+      <c r="C27" s="129"/>
+      <c r="D27" s="129"/>
+      <c r="E27" s="130"/>
+      <c r="G27" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="H27" s="122"/>
-      <c r="I27" s="122"/>
-      <c r="J27" s="134"/>
-      <c r="K27" s="135"/>
+      <c r="H27" s="129"/>
+      <c r="I27" s="129"/>
+      <c r="J27" s="141"/>
+      <c r="K27" s="142"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="41" t="s">
@@ -7542,7 +7639,7 @@
       <c r="C28" t="s">
         <v>118</v>
       </c>
-      <c r="E28" s="112"/>
+      <c r="E28" s="119"/>
       <c r="G28" s="41" t="s">
         <v>110</v>
       </c>
@@ -7552,7 +7649,7 @@
       <c r="I28" t="s">
         <v>118</v>
       </c>
-      <c r="K28" s="114"/>
+      <c r="K28" s="121"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -7564,7 +7661,7 @@
       <c r="C29" t="s">
         <v>117</v>
       </c>
-      <c r="E29" s="112"/>
+      <c r="E29" s="119"/>
       <c r="G29" t="s">
         <v>111</v>
       </c>
@@ -7574,7 +7671,7 @@
       <c r="I29" t="s">
         <v>117</v>
       </c>
-      <c r="K29" s="114"/>
+      <c r="K29" s="121"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="25" t="s">
@@ -7586,7 +7683,7 @@
       <c r="C30" t="s">
         <v>116</v>
       </c>
-      <c r="E30" s="112"/>
+      <c r="E30" s="119"/>
       <c r="G30" s="25" t="s">
         <v>109</v>
       </c>
@@ -7596,7 +7693,7 @@
       <c r="I30" t="s">
         <v>116</v>
       </c>
-      <c r="K30" s="114"/>
+      <c r="K30" s="121"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="25" t="s">
@@ -7608,7 +7705,7 @@
       <c r="C31" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="112"/>
+      <c r="E31" s="119"/>
       <c r="G31" s="25" t="s">
         <v>113</v>
       </c>
@@ -7618,7 +7715,7 @@
       <c r="I31" t="s">
         <v>115</v>
       </c>
-      <c r="K31" s="114"/>
+      <c r="K31" s="121"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="27" t="s">
@@ -7629,7 +7726,7 @@
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
-      <c r="E32" s="113"/>
+      <c r="E32" s="120"/>
       <c r="G32" s="27" t="s">
         <v>122</v>
       </c>
@@ -7638,7 +7735,7 @@
       </c>
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
-      <c r="K32" s="114"/>
+      <c r="K32" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -7697,118 +7794,118 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:26" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="149" t="s">
+      <c r="B1" s="156" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="150"/>
-      <c r="I1" s="150"/>
-      <c r="J1" s="150"/>
-      <c r="K1" s="150"/>
-      <c r="L1" s="150"/>
-      <c r="M1" s="150"/>
-      <c r="N1" s="150"/>
-      <c r="O1" s="150"/>
-      <c r="P1" s="150"/>
-      <c r="Q1" s="150"/>
-      <c r="R1" s="150"/>
-      <c r="S1" s="150"/>
-      <c r="T1" s="150"/>
-      <c r="U1" s="150"/>
-      <c r="V1" s="150"/>
-      <c r="W1" s="150"/>
-      <c r="X1" s="150"/>
-      <c r="Y1" s="150"/>
-      <c r="Z1" s="151"/>
+      <c r="C1" s="157"/>
+      <c r="D1" s="157"/>
+      <c r="E1" s="157"/>
+      <c r="F1" s="157"/>
+      <c r="G1" s="157"/>
+      <c r="H1" s="157"/>
+      <c r="I1" s="157"/>
+      <c r="J1" s="157"/>
+      <c r="K1" s="157"/>
+      <c r="L1" s="157"/>
+      <c r="M1" s="157"/>
+      <c r="N1" s="157"/>
+      <c r="O1" s="157"/>
+      <c r="P1" s="157"/>
+      <c r="Q1" s="157"/>
+      <c r="R1" s="157"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="157"/>
+      <c r="W1" s="157"/>
+      <c r="X1" s="157"/>
+      <c r="Y1" s="157"/>
+      <c r="Z1" s="158"/>
     </row>
     <row r="2" spans="2:26" s="19" customFormat="1" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="159" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
-      <c r="I2" s="153"/>
-      <c r="J2" s="153"/>
-      <c r="K2" s="153"/>
-      <c r="L2" s="153"/>
-      <c r="M2" s="153"/>
-      <c r="N2" s="153"/>
-      <c r="O2" s="153"/>
-      <c r="P2" s="153"/>
-      <c r="Q2" s="153"/>
-      <c r="R2" s="153"/>
-      <c r="S2" s="153"/>
-      <c r="T2" s="153"/>
-      <c r="U2" s="153"/>
-      <c r="V2" s="153"/>
-      <c r="W2" s="153"/>
-      <c r="X2" s="153"/>
-      <c r="Y2" s="153"/>
-      <c r="Z2" s="154"/>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="160"/>
+      <c r="H2" s="160"/>
+      <c r="I2" s="160"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160"/>
+      <c r="L2" s="160"/>
+      <c r="M2" s="160"/>
+      <c r="N2" s="160"/>
+      <c r="O2" s="160"/>
+      <c r="P2" s="160"/>
+      <c r="Q2" s="160"/>
+      <c r="R2" s="160"/>
+      <c r="S2" s="160"/>
+      <c r="T2" s="160"/>
+      <c r="U2" s="160"/>
+      <c r="V2" s="160"/>
+      <c r="W2" s="160"/>
+      <c r="X2" s="160"/>
+      <c r="Y2" s="160"/>
+      <c r="Z2" s="161"/>
     </row>
     <row r="3" spans="2:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="155" t="s">
+      <c r="B3" s="162" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
-      <c r="J3" s="156"/>
-      <c r="K3" s="156"/>
-      <c r="L3" s="156"/>
-      <c r="M3" s="156"/>
-      <c r="N3" s="156"/>
-      <c r="O3" s="156"/>
-      <c r="P3" s="156"/>
-      <c r="Q3" s="156"/>
-      <c r="R3" s="156"/>
-      <c r="S3" s="156"/>
-      <c r="T3" s="156"/>
-      <c r="U3" s="156"/>
-      <c r="V3" s="156"/>
-      <c r="W3" s="156"/>
-      <c r="X3" s="156"/>
-      <c r="Y3" s="156"/>
-      <c r="Z3" s="157"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="163"/>
+      <c r="I3" s="163"/>
+      <c r="J3" s="163"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="163"/>
+      <c r="M3" s="163"/>
+      <c r="N3" s="163"/>
+      <c r="O3" s="163"/>
+      <c r="P3" s="163"/>
+      <c r="Q3" s="163"/>
+      <c r="R3" s="163"/>
+      <c r="S3" s="163"/>
+      <c r="T3" s="163"/>
+      <c r="U3" s="163"/>
+      <c r="V3" s="163"/>
+      <c r="W3" s="163"/>
+      <c r="X3" s="163"/>
+      <c r="Y3" s="163"/>
+      <c r="Z3" s="164"/>
     </row>
     <row r="4" spans="2:26" s="19" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="158"/>
-      <c r="C4" s="159"/>
-      <c r="D4" s="159"/>
-      <c r="E4" s="159"/>
-      <c r="F4" s="159"/>
-      <c r="G4" s="159"/>
-      <c r="H4" s="159"/>
-      <c r="I4" s="159"/>
-      <c r="J4" s="159"/>
-      <c r="K4" s="159"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="159"/>
-      <c r="N4" s="159"/>
-      <c r="O4" s="159"/>
-      <c r="P4" s="159"/>
-      <c r="Q4" s="159"/>
-      <c r="R4" s="159"/>
-      <c r="S4" s="159"/>
-      <c r="T4" s="159"/>
-      <c r="U4" s="159"/>
-      <c r="V4" s="159"/>
-      <c r="W4" s="159"/>
-      <c r="X4" s="159"/>
-      <c r="Y4" s="159"/>
-      <c r="Z4" s="160"/>
+      <c r="B4" s="165"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="166"/>
+      <c r="H4" s="166"/>
+      <c r="I4" s="166"/>
+      <c r="J4" s="166"/>
+      <c r="K4" s="166"/>
+      <c r="L4" s="166"/>
+      <c r="M4" s="166"/>
+      <c r="N4" s="166"/>
+      <c r="O4" s="166"/>
+      <c r="P4" s="166"/>
+      <c r="Q4" s="166"/>
+      <c r="R4" s="166"/>
+      <c r="S4" s="166"/>
+      <c r="T4" s="166"/>
+      <c r="U4" s="166"/>
+      <c r="V4" s="166"/>
+      <c r="W4" s="166"/>
+      <c r="X4" s="166"/>
+      <c r="Y4" s="166"/>
+      <c r="Z4" s="167"/>
     </row>
     <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="33"/>
@@ -7949,60 +8046,60 @@
       <c r="Z11" s="40"/>
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B12" s="143" t="s">
+      <c r="B12" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="C12" s="144"/>
-      <c r="D12" s="144"/>
-      <c r="E12" s="144"/>
-      <c r="F12" s="144"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="144"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="144"/>
-      <c r="Q12" s="144"/>
-      <c r="R12" s="144"/>
-      <c r="S12" s="144"/>
-      <c r="T12" s="144"/>
-      <c r="U12" s="144"/>
-      <c r="V12" s="144"/>
-      <c r="W12" s="144"/>
-      <c r="X12" s="144"/>
-      <c r="Y12" s="144"/>
-      <c r="Z12" s="145"/>
+      <c r="C12" s="151"/>
+      <c r="D12" s="151"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="151"/>
+      <c r="G12" s="151"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="151"/>
+      <c r="J12" s="151"/>
+      <c r="K12" s="151"/>
+      <c r="L12" s="151"/>
+      <c r="M12" s="151"/>
+      <c r="N12" s="151"/>
+      <c r="O12" s="151"/>
+      <c r="P12" s="151"/>
+      <c r="Q12" s="151"/>
+      <c r="R12" s="151"/>
+      <c r="S12" s="151"/>
+      <c r="T12" s="151"/>
+      <c r="U12" s="151"/>
+      <c r="V12" s="151"/>
+      <c r="W12" s="151"/>
+      <c r="X12" s="151"/>
+      <c r="Y12" s="151"/>
+      <c r="Z12" s="152"/>
     </row>
     <row r="13" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="146"/>
-      <c r="C13" s="147"/>
-      <c r="D13" s="147"/>
-      <c r="E13" s="147"/>
-      <c r="F13" s="147"/>
-      <c r="G13" s="147"/>
-      <c r="H13" s="147"/>
-      <c r="I13" s="147"/>
-      <c r="J13" s="147"/>
-      <c r="K13" s="147"/>
-      <c r="L13" s="147"/>
-      <c r="M13" s="147"/>
-      <c r="N13" s="147"/>
-      <c r="O13" s="147"/>
-      <c r="P13" s="147"/>
-      <c r="Q13" s="147"/>
-      <c r="R13" s="147"/>
-      <c r="S13" s="147"/>
-      <c r="T13" s="147"/>
-      <c r="U13" s="147"/>
-      <c r="V13" s="147"/>
-      <c r="W13" s="147"/>
-      <c r="X13" s="147"/>
-      <c r="Y13" s="147"/>
-      <c r="Z13" s="148"/>
+      <c r="B13" s="153"/>
+      <c r="C13" s="154"/>
+      <c r="D13" s="154"/>
+      <c r="E13" s="154"/>
+      <c r="F13" s="154"/>
+      <c r="G13" s="154"/>
+      <c r="H13" s="154"/>
+      <c r="I13" s="154"/>
+      <c r="J13" s="154"/>
+      <c r="K13" s="154"/>
+      <c r="L13" s="154"/>
+      <c r="M13" s="154"/>
+      <c r="N13" s="154"/>
+      <c r="O13" s="154"/>
+      <c r="P13" s="154"/>
+      <c r="Q13" s="154"/>
+      <c r="R13" s="154"/>
+      <c r="S13" s="154"/>
+      <c r="T13" s="154"/>
+      <c r="U13" s="154"/>
+      <c r="V13" s="154"/>
+      <c r="W13" s="154"/>
+      <c r="X13" s="154"/>
+      <c r="Y13" s="154"/>
+      <c r="Z13" s="155"/>
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="33"/>
@@ -8143,60 +8240,60 @@
       <c r="Z20" s="40"/>
     </row>
     <row r="21" spans="2:26" x14ac:dyDescent="0.25">
-      <c r="B21" s="143" t="s">
+      <c r="B21" s="150" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="144"/>
-      <c r="D21" s="144"/>
-      <c r="E21" s="144"/>
-      <c r="F21" s="144"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
-      <c r="K21" s="144"/>
-      <c r="L21" s="144"/>
-      <c r="M21" s="144"/>
-      <c r="N21" s="144"/>
-      <c r="O21" s="144"/>
-      <c r="P21" s="144"/>
-      <c r="Q21" s="144"/>
-      <c r="R21" s="144"/>
-      <c r="S21" s="144"/>
-      <c r="T21" s="144"/>
-      <c r="U21" s="144"/>
-      <c r="V21" s="144"/>
-      <c r="W21" s="144"/>
-      <c r="X21" s="144"/>
-      <c r="Y21" s="144"/>
-      <c r="Z21" s="145"/>
+      <c r="C21" s="151"/>
+      <c r="D21" s="151"/>
+      <c r="E21" s="151"/>
+      <c r="F21" s="151"/>
+      <c r="G21" s="151"/>
+      <c r="H21" s="151"/>
+      <c r="I21" s="151"/>
+      <c r="J21" s="151"/>
+      <c r="K21" s="151"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="151"/>
+      <c r="N21" s="151"/>
+      <c r="O21" s="151"/>
+      <c r="P21" s="151"/>
+      <c r="Q21" s="151"/>
+      <c r="R21" s="151"/>
+      <c r="S21" s="151"/>
+      <c r="T21" s="151"/>
+      <c r="U21" s="151"/>
+      <c r="V21" s="151"/>
+      <c r="W21" s="151"/>
+      <c r="X21" s="151"/>
+      <c r="Y21" s="151"/>
+      <c r="Z21" s="152"/>
     </row>
     <row r="22" spans="2:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="146"/>
-      <c r="C22" s="147"/>
-      <c r="D22" s="147"/>
-      <c r="E22" s="147"/>
-      <c r="F22" s="147"/>
-      <c r="G22" s="147"/>
-      <c r="H22" s="147"/>
-      <c r="I22" s="147"/>
-      <c r="J22" s="147"/>
-      <c r="K22" s="147"/>
-      <c r="L22" s="147"/>
-      <c r="M22" s="147"/>
-      <c r="N22" s="147"/>
-      <c r="O22" s="147"/>
-      <c r="P22" s="147"/>
-      <c r="Q22" s="147"/>
-      <c r="R22" s="147"/>
-      <c r="S22" s="147"/>
-      <c r="T22" s="147"/>
-      <c r="U22" s="147"/>
-      <c r="V22" s="147"/>
-      <c r="W22" s="147"/>
-      <c r="X22" s="147"/>
-      <c r="Y22" s="147"/>
-      <c r="Z22" s="148"/>
+      <c r="B22" s="153"/>
+      <c r="C22" s="154"/>
+      <c r="D22" s="154"/>
+      <c r="E22" s="154"/>
+      <c r="F22" s="154"/>
+      <c r="G22" s="154"/>
+      <c r="H22" s="154"/>
+      <c r="I22" s="154"/>
+      <c r="J22" s="154"/>
+      <c r="K22" s="154"/>
+      <c r="L22" s="154"/>
+      <c r="M22" s="154"/>
+      <c r="N22" s="154"/>
+      <c r="O22" s="154"/>
+      <c r="P22" s="154"/>
+      <c r="Q22" s="154"/>
+      <c r="R22" s="154"/>
+      <c r="S22" s="154"/>
+      <c r="T22" s="154"/>
+      <c r="U22" s="154"/>
+      <c r="V22" s="154"/>
+      <c r="W22" s="154"/>
+      <c r="X22" s="154"/>
+      <c r="Y22" s="154"/>
+      <c r="Z22" s="155"/>
     </row>
     <row r="23" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B23" s="33"/>
@@ -8530,7 +8627,7 @@
       <c r="D10" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="E10" s="173" t="s">
+      <c r="E10" s="85" t="s">
         <v>286</v>
       </c>
     </row>
@@ -8541,29 +8638,29 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F332D551-BFDC-4D6A-9D91-6841C7A71890}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="90" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" style="90" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="89" t="s">
         <v>36</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -8575,19 +8672,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+        <v>297</v>
+      </c>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="3"/>
+      <c r="C3" s="87"/>
       <c r="D3" s="3"/>
       <c r="E3" s="82" t="s">
         <v>275</v>
@@ -8595,85 +8692,85 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="87" t="s">
         <v>266</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>288</v>
+      <c r="E4" s="82" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="87" t="s">
         <v>267</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>272</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="87" t="s">
         <v>276</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>290</v>
+      <c r="E6" s="178" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="87" t="s">
         <v>44</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>272</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>287</v>
+        <v>314</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="87" t="s">
         <v>274</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>272</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>287</v>
+        <v>315</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="87" t="s">
         <v>273</v>
       </c>
       <c r="D9" s="3" t="s">
@@ -8685,155 +8782,900 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>282</v>
+      <c r="C10" s="87" t="s">
+        <v>304</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>272</v>
       </c>
       <c r="E10" s="83" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="83"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C11" s="87" t="s">
+        <v>305</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="82" t="s">
-        <v>275</v>
+      <c r="B12" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C12" s="87" t="s">
+        <v>306</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="83" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>266</v>
+      <c r="B13" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>312</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>288</v>
+      <c r="E13" s="83" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>267</v>
+      <c r="B14" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C14" s="87" t="s">
+        <v>307</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>289</v>
+      <c r="E14" s="83" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>290</v>
-      </c>
+      <c r="A15" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="B15" s="87"/>
+      <c r="C15" s="87"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>287</v>
+      <c r="B16" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="87"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="82" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>274</v>
+      <c r="C17" s="87" t="s">
+        <v>266</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>287</v>
+      <c r="E17" s="82" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>273</v>
+      <c r="B18" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="87" t="s">
+        <v>267</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="E18" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E22" s="83" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="45"/>
-      <c r="B19" s="45" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="87" t="s">
         <v>280</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C23" s="87" t="s">
+        <v>307</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E23" s="83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="B24" s="87"/>
+      <c r="C24" s="87"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="2"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="87"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E26" s="82" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
+      <c r="B27" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3"/>
+      <c r="B29" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3"/>
+      <c r="B30" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E31" s="83" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C32" s="87" t="s">
+        <v>312</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E32" s="83" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="87"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="87"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E35" s="82" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="3"/>
+      <c r="B36" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="3"/>
+      <c r="B37" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="3"/>
+      <c r="B38" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="3"/>
+      <c r="B39" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E40" s="83" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="3"/>
+      <c r="B41" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C41" s="87" t="s">
+        <v>307</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E41" s="83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="3"/>
+      <c r="B43" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="87"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A44" s="3"/>
+      <c r="B44" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E44" s="86" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" s="3"/>
+      <c r="B45" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C45" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E45" s="43" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="3"/>
+      <c r="B46" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E46" s="88" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A47" s="3"/>
+      <c r="B47" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E47" s="43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="3"/>
+      <c r="B48" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E48" s="43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="3"/>
+      <c r="B49" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E49" s="83" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="3"/>
+      <c r="B50" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C50" s="87" t="s">
+        <v>304</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E50" s="83" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C51" s="87" t="s">
+        <v>305</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E51" s="83" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="3"/>
+      <c r="B52" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C52" s="87" t="s">
+        <v>306</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E52" s="83" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C53" s="87" t="s">
+        <v>312</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E53" s="83" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="3"/>
+      <c r="B54" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C54" s="87" t="s">
+        <v>307</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E54" s="83" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B55" s="87"/>
+      <c r="C55" s="87"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="2"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="3"/>
+      <c r="B56" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="87"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="3"/>
+      <c r="B57" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C57" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="3"/>
+      <c r="B58" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C58" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="3"/>
+      <c r="B59" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C59" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="3"/>
+      <c r="B60" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C60" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="3"/>
+      <c r="B61" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="3"/>
+      <c r="B62" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E62" s="83" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="3"/>
+      <c r="B63" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C63" s="87" t="s">
+        <v>282</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E63" s="83" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B64" s="87"/>
+      <c r="C64" s="87"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="83"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3"/>
+      <c r="B65" s="87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C65" s="87"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="82" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3"/>
+      <c r="B66" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="87" t="s">
+        <v>266</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="3"/>
+      <c r="B67" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C67" s="87" t="s">
+        <v>267</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="3"/>
+      <c r="B68" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C68" s="87" t="s">
+        <v>276</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3"/>
+      <c r="B69" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C69" s="87" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3"/>
+      <c r="B70" s="87" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="87" t="s">
+        <v>274</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3"/>
+      <c r="B71" s="87" t="s">
+        <v>45</v>
+      </c>
+      <c r="C71" s="87" t="s">
+        <v>273</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E71" s="83" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="45"/>
+      <c r="B72" s="87" t="s">
+        <v>280</v>
+      </c>
+      <c r="C72" s="87" t="s">
         <v>281</v>
       </c>
-      <c r="D19" s="45" t="s">
+      <c r="D72" s="45" t="s">
         <v>272</v>
       </c>
-      <c r="E19" s="83" t="s">
+      <c r="E72" s="83" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="171"/>
-      <c r="B20" s="171"/>
-      <c r="C20" s="171"/>
-      <c r="D20" s="171"/>
-      <c r="E20" s="172"/>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="84"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" xr:uid="{5E58ABFA-7F07-45A9-BD5A-8D518C2E12CB}"/>
-    <hyperlink ref="E15" r:id="rId2" xr:uid="{7CD0E5F5-D8AB-4D8A-8528-5FFABE73A259}"/>
+    <hyperlink ref="E68" r:id="rId1" xr:uid="{7CD0E5F5-D8AB-4D8A-8528-5FFABE73A259}"/>
+    <hyperlink ref="E59" r:id="rId2" xr:uid="{5E58ABFA-7F07-45A9-BD5A-8D518C2E12CB}"/>
+    <hyperlink ref="E19" r:id="rId3" xr:uid="{B6BA1F80-62B9-48D0-9A9B-1E400DC57C24}"/>
+    <hyperlink ref="E28" r:id="rId4" xr:uid="{83689B93-41E7-4BD6-8881-CE6DFB843209}"/>
+    <hyperlink ref="E37" r:id="rId5" xr:uid="{487FE0CE-DEE4-4C4F-A3C9-4F082335178B}"/>
+    <hyperlink ref="E46" r:id="rId6" display="lethu@testauuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuuutomation.co.za" xr:uid="{186E6E9F-40A0-4A6C-9F33-8B67F5F20254}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9283,7 +10125,7 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9313,13 +10155,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="164" t="s">
+      <c r="A2" s="171" t="s">
         <v>251</v>
       </c>
-      <c r="B2" s="165"/>
-      <c r="C2" s="165"/>
-      <c r="D2" s="165"/>
-      <c r="E2" s="166"/>
+      <c r="B2" s="172"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="172"/>
+      <c r="E2" s="173"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -9367,13 +10209,13 @@
       <c r="E5" s="80"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="161" t="s">
+      <c r="A6" s="168" t="s">
         <v>264</v>
       </c>
-      <c r="B6" s="162"/>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="163"/>
+      <c r="B6" s="169"/>
+      <c r="C6" s="169"/>
+      <c r="D6" s="169"/>
+      <c r="E6" s="170"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="71" t="s">
@@ -9482,13 +10324,13 @@
       <c r="E13" s="80"/>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="161" t="s">
+      <c r="A14" s="168" t="s">
         <v>263</v>
       </c>
-      <c r="B14" s="162"/>
-      <c r="C14" s="162"/>
-      <c r="D14" s="162"/>
-      <c r="E14" s="163"/>
+      <c r="B14" s="169"/>
+      <c r="C14" s="169"/>
+      <c r="D14" s="169"/>
+      <c r="E14" s="170"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="71" t="s">
@@ -9716,7 +10558,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9769,18 +10611,18 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="167" t="s">
+      <c r="A2" s="174" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="167"/>
-      <c r="C2" s="167"/>
-      <c r="D2" s="167"/>
-      <c r="E2" s="167"/>
-      <c r="F2" s="167"/>
-      <c r="G2" s="167"/>
-      <c r="H2" s="167"/>
-      <c r="I2" s="167"/>
-      <c r="J2" s="167"/>
+      <c r="B2" s="174"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
+      <c r="H2" s="174"/>
+      <c r="I2" s="174"/>
+      <c r="J2" s="174"/>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="71" t="s">

</xml_diff>